<commit_message>
refactor backend code and wording and change returned type
</commit_message>
<xml_diff>
--- a/dd5-generator/src/treasureGenerator/files/treasureGen.xlsx
+++ b/dd5-generator/src/treasureGenerator/files/treasureGen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DDGen\DD5Generator\dd5-generator\src\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yann\Documents\DEV\DnD\DD5-Generator\dd5-generator\src\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E134F3-17DA-4047-8776-003F9B5D98CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F808D53-EB5E-4E1F-959C-A5C1B4E678C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
   <si>
     <t>1d20</t>
   </si>
@@ -45,97 +45,31 @@
     <t>17 et +</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>1 objet à 25 po</t>
-  </si>
-  <si>
-    <t>2d6 (7) gemmes à 50 po</t>
-  </si>
-  <si>
-    <t>1 objet à 750 po</t>
-  </si>
-  <si>
-    <t>3d6 (10) gemmes à 500 po</t>
-  </si>
-  <si>
-    <t>1 objet à 7500 po</t>
-  </si>
-  <si>
-    <t>2d6 (7) gemmes à 10 po</t>
-  </si>
-  <si>
-    <t>1d4 (2) objets à 25 po</t>
-  </si>
-  <si>
-    <t>3d6 (10) gemmes à 50 po</t>
-  </si>
-  <si>
-    <t>1 objet à 2500 po</t>
-  </si>
-  <si>
-    <t>3d6 (10) gemmes à 1000 po</t>
-  </si>
-  <si>
-    <t>1d6 (3) gemmes à 100 po</t>
-  </si>
-  <si>
-    <t>1d4 (2) objets à 750 po</t>
-  </si>
-  <si>
-    <t>2d6 (7) gemmes à 1000 po</t>
-  </si>
-  <si>
-    <t>1d4 (2) objets à 7500 po</t>
-  </si>
-  <si>
-    <t>14-16</t>
-  </si>
-  <si>
-    <t>1d6 (3) gemmes à 50 po</t>
-  </si>
-  <si>
-    <t>2d4 (5) gemmes à 50 po</t>
-  </si>
-  <si>
-    <t>1d4 (2) objets à 2500 po</t>
-  </si>
-  <si>
-    <t>1d6 (3) gemmes à 5000 po</t>
-  </si>
-  <si>
-    <t>17-19</t>
-  </si>
-  <si>
-    <t>1 objet à 250 po</t>
-  </si>
-  <si>
-    <t>2d4 (5) objets à 750 po</t>
-  </si>
-  <si>
-    <t>2d4 (5) objets à 7500 po</t>
-  </si>
-  <si>
-    <t>2d6 (7) gemmes à 100 po</t>
-  </si>
-  <si>
-    <t>3d6 (10) gemmes à 100 po</t>
-  </si>
-  <si>
-    <t>1d8 (4) gemmes à 5000 po</t>
-  </si>
-  <si>
-    <t>1-2</t>
-  </si>
-  <si>
-    <t>3-5</t>
-  </si>
-  <si>
-    <t>6-9</t>
-  </si>
-  <si>
-    <t>10-13</t>
+    <t>15-18</t>
+  </si>
+  <si>
+    <t>19-20</t>
+  </si>
+  <si>
+    <t>01-05</t>
+  </si>
+  <si>
+    <t>11-14</t>
+  </si>
+  <si>
+    <t>06-10</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>ABCD</t>
+  </si>
+  <si>
+    <t>ABC</t>
   </si>
 </sst>
 </file>
@@ -152,10 +86,11 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Roboto"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Roboto"/>
@@ -163,7 +98,7 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Roboto"/>
     </font>
   </fonts>
@@ -188,7 +123,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
+        <fgColor theme="5" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -205,29 +140,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,181 +444,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" customWidth="1"/>
-    <col min="4" max="4" width="27.88671875" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" customWidth="1"/>
-    <col min="6" max="6" width="28.44140625" customWidth="1"/>
+    <col min="2" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>20</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>